<commit_message>
point : desgine comp (close #10)
</commit_message>
<xml_diff>
--- a/機械設計/_BOM/CGA75.xlsx
+++ b/機械設計/_BOM/CGA75.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\2022-KawasakiRobot\機械設計\_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7058D22D-EB27-492F-8A03-2B063FF16855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{68E68E41-44E0-401B-B202-65540B792A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17970" yWindow="-2220" windowWidth="14400" windowHeight="10845" xr2:uid="{D28DC254-7CB2-4F8B-BA1A-AA3695AF23E3}"/>
+    <workbookView xWindow="42120" yWindow="6870" windowWidth="14400" windowHeight="10845" xr2:uid="{F5E0205B-AC19-4B3E-9601-86D001EE6C73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
-    <customWorkbookView name="DESKTOP-1 - 個人用ビュー" guid="{F1BCFEA6-D08E-48A7-9A05-A3D36ADA41AE}" mergeInterval="0" personalView="1" xWindow="-1198" yWindow="-148" windowWidth="960" windowHeight="723" activeSheetId="1"/>
+    <customWorkbookView name="DESKTOP-1 - 個人用ビュー" guid="{5B41751C-FDD5-4480-99FC-823345FA3423}" mergeInterval="0" personalView="1" xWindow="2808" yWindow="458" windowWidth="960" windowHeight="723" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -206,7 +206,7 @@
     <t>B6802ZZ</t>
   </si>
   <si>
-    <t>CBSTSR4-5</t>
+    <t>CBSTSR4-8</t>
   </si>
   <si>
     <t>SUS304相当</t>
@@ -296,8 +296,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{5A79B6DD-C486-4AFD-ACBD-58B5B69CF71F}">
-  <header guid="{5A79B6DD-C486-4AFD-ACBD-58B5B69CF71F}" dateTime="2023-07-13T20:32:14" maxSheetId="2" userName="DESKTOP-1" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B3A3B874-15C7-48F6-90E3-6F9335DD0D98}">
+  <header guid="{B3A3B874-15C7-48F6-90E3-6F9335DD0D98}" dateTime="2023-07-16T16:25:43" maxSheetId="2" userName="DESKTOP-1" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -609,7 +609,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A4C562-8C90-483D-AFF8-E4052FD73888}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1871CB98-8518-4B3B-84CC-2068ACE49A4C}">
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1232,7 +1232,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F1BCFEA6-D08E-48A7-9A05-A3D36ADA41AE}">
+    <customSheetView guid="{5B41751C-FDD5-4480-99FC-823345FA3423}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
     </customSheetView>

</xml_diff>